<commit_message>
tidied measures folder, updated task parameters file
</commit_message>
<xml_diff>
--- a/measures/word stimuli and task parameters.xlsx
+++ b/measures/word stimuli and task parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/irap-reliability-meta-analysis/measures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853DBF87-40FD-E34A-B9E0-6E60F477DA23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE34D32D-4FF0-EF48-8D4D-51BA320C1C76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="460" windowWidth="23520" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="215">
   <si>
     <t>Religion</t>
   </si>
@@ -217,9 +217,6 @@
     <t>See "image stimuli" folder for images</t>
   </si>
   <si>
-    <t>Only either male or female category stimuli were used in a given IRAP. Category stimuli were used in a vignette that participants read prior to completing the IRAP (see Vignettes folder).</t>
-  </si>
-  <si>
     <t>Hillary Clinton</t>
   </si>
   <si>
@@ -660,6 +657,21 @@
   <si>
     <t>See "image stimuli" folder for images 
 HAVE I CORRECTLY ASSIGNED RACE 1-3???</t>
+  </si>
+  <si>
+    <t>Only either male or female category stimuli were used in a given IRAP, gender matched to the participant. Category stimuli were used in a vignette that participants read prior to completing the IRAP (see Vignettes folder).</t>
+  </si>
+  <si>
+    <t>forceful, logical, dominant, forceful, logical, dominant</t>
+  </si>
+  <si>
+    <t>gentle, emotional,  sensitive, gentle, emotional,  sensitive</t>
+  </si>
+  <si>
+    <t>males, mean</t>
+  </si>
+  <si>
+    <t>females, women</t>
   </si>
 </sst>
 </file>
@@ -875,7 +887,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -932,9 +944,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1420,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1434,20 +1443,20 @@
     <col min="9" max="9" width="23" style="9" customWidth="1"/>
     <col min="10" max="11" width="25" style="1" customWidth="1"/>
     <col min="12" max="13" width="29" style="1" customWidth="1"/>
-    <col min="14" max="15" width="23.83203125" style="23" customWidth="1"/>
+    <col min="14" max="15" width="23.83203125" style="22" customWidth="1"/>
     <col min="16" max="16" width="69.1640625" style="9" customWidth="1"/>
     <col min="17" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>18</v>
@@ -1456,7 +1465,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>54</v>
@@ -1480,10 +1489,10 @@
         <v>24</v>
       </c>
       <c r="N1" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>89</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>61</v>
@@ -1536,16 +1545,16 @@
     </row>
     <row r="3" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="F3" s="10">
         <v>78</v>
@@ -1560,16 +1569,16 @@
         <v>15</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="L3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="N3" s="19" t="b">
         <v>1</v>
@@ -1580,19 +1589,19 @@
     </row>
     <row r="4" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="11">
         <v>80</v>
@@ -1604,19 +1613,19 @@
         <v>17</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="L4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="N4" s="19" t="b">
         <v>1</v>
@@ -1627,19 +1636,19 @@
     </row>
     <row r="5" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="9">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>107</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="F5" s="11">
         <v>80</v>
@@ -1651,19 +1660,19 @@
         <v>17</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="N5" s="19" t="b">
         <v>1</v>
@@ -1674,19 +1683,19 @@
     </row>
     <row r="6" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="9">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D6" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>91</v>
       </c>
       <c r="F6" s="11">
         <v>80</v>
@@ -1698,19 +1707,19 @@
         <v>17</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="N6" s="19" t="b">
         <v>1</v>
@@ -1721,19 +1730,19 @@
     </row>
     <row r="7" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="9">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="F7" s="11">
         <v>80</v>
@@ -1745,19 +1754,19 @@
         <v>17</v>
       </c>
       <c r="I7" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="N7" s="19" t="b">
         <v>1</v>
@@ -1774,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1792,7 +1801,7 @@
         <v>17</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>38</v>
@@ -1821,7 +1830,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -1839,7 +1848,7 @@
         <v>17</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>38</v>
@@ -1868,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -1886,7 +1895,7 @@
         <v>17</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>39</v>
@@ -1909,17 +1918,17 @@
     </row>
     <row r="11" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>121</v>
       </c>
       <c r="F11" s="10">
         <v>80</v>
@@ -1931,19 +1940,19 @@
         <v>17</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="L11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="N11" s="19" t="b">
         <v>1</v>
@@ -1957,11 +1966,11 @@
     </row>
     <row r="12" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
@@ -2002,19 +2011,19 @@
     </row>
     <row r="13" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>128</v>
       </c>
       <c r="F13" s="12">
         <v>80</v>
@@ -2029,40 +2038,40 @@
         <v>15</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>67</v>
+        <v>213</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>214</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>70</v>
+        <v>211</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="N13" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" s="21" t="b">
+        <v>212</v>
+      </c>
+      <c r="N13" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="P13" s="22"/>
+      <c r="P13" s="21"/>
     </row>
     <row r="14" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="F14" s="10">
         <v>78</v>
@@ -2077,16 +2086,16 @@
         <v>15</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="L14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="N14" s="19" t="b">
         <v>1</v>
@@ -2097,11 +2106,11 @@
     </row>
     <row r="15" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -2116,7 +2125,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
@@ -2166,19 +2175,19 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="F17" s="10">
         <v>78</v>
@@ -2193,13 +2202,13 @@
         <v>15</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="L17" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="M17" s="19" t="s">
         <v>60</v>
@@ -2210,25 +2219,25 @@
       <c r="O17" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="P17" s="4" t="s">
-        <v>63</v>
+      <c r="P17" s="19" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="F18" s="10">
         <v>78</v>
@@ -2243,16 +2252,16 @@
         <v>15</v>
       </c>
       <c r="J18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="M18" s="19" t="s">
         <v>144</v>
-      </c>
-      <c r="M18" s="19" t="s">
-        <v>145</v>
       </c>
       <c r="N18" s="19" t="b">
         <v>1</v>
@@ -2260,25 +2269,25 @@
       <c r="O18" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="P18" s="4" t="s">
-        <v>63</v>
+      <c r="P18" s="19" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="F19" s="10">
         <v>78</v>
@@ -2293,16 +2302,16 @@
         <v>15</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="L19" s="19" t="s">
-        <v>144</v>
-      </c>
       <c r="M19" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N19" s="19" t="b">
         <v>1</v>
@@ -2310,25 +2319,25 @@
       <c r="O19" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="P19" s="4" t="s">
-        <v>63</v>
+      <c r="P19" s="19" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>148</v>
       </c>
       <c r="F20" s="11">
         <v>78</v>
@@ -2343,16 +2352,16 @@
         <v>15</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="N20" s="19" t="b">
         <v>1</v>
@@ -2360,22 +2369,23 @@
       <c r="O20" s="19" t="b">
         <v>0</v>
       </c>
+      <c r="P20" s="22"/>
     </row>
     <row r="21" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>157</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>158</v>
       </c>
       <c r="F21" s="11">
         <v>78</v>
@@ -2390,16 +2400,16 @@
         <v>15</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="N21" s="19" t="b">
         <v>1</v>
@@ -2410,19 +2420,19 @@
     </row>
     <row r="22" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="F22" s="11">
         <v>78</v>
@@ -2437,16 +2447,16 @@
         <v>15</v>
       </c>
       <c r="J22" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="N22" s="19" t="b">
         <v>1</v>
@@ -2457,19 +2467,19 @@
     </row>
     <row r="23" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>176</v>
       </c>
       <c r="F23" s="11">
         <v>78</v>
@@ -2484,16 +2494,16 @@
         <v>15</v>
       </c>
       <c r="J23" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="N23" s="19" t="b">
         <v>1</v>
@@ -2504,19 +2514,19 @@
     </row>
     <row r="24" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>174</v>
       </c>
       <c r="F24" s="11">
         <v>78</v>
@@ -2531,16 +2541,16 @@
         <v>15</v>
       </c>
       <c r="J24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="N24" s="19" t="b">
         <v>1</v>
@@ -2551,13 +2561,13 @@
     </row>
     <row r="25" spans="1:16" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>3</v>
@@ -2598,13 +2608,13 @@
     </row>
     <row r="26" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B26" s="3">
         <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
@@ -2622,7 +2632,7 @@
         <v>17</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>55</v>
@@ -2642,19 +2652,19 @@
       <c r="O26" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="P26" s="4" t="s">
+      <c r="P26" s="19" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" s="3">
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>13</v>
@@ -2672,7 +2682,7 @@
         <v>17</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>55</v>
@@ -2693,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -2743,16 +2753,16 @@
     </row>
     <row r="29" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>82</v>
       </c>
       <c r="F29" s="10">
         <v>78</v>
@@ -2767,10 +2777,10 @@
         <v>15</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>41</v>
@@ -2787,17 +2797,17 @@
     </row>
     <row r="30" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="E30" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>114</v>
       </c>
       <c r="F30" s="10">
         <v>80</v>
@@ -2812,16 +2822,16 @@
         <v>15</v>
       </c>
       <c r="J30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K30" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="L30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="N30" s="19" t="b">
         <v>1</v>
@@ -2835,17 +2845,17 @@
     </row>
     <row r="31" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B31" s="8">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="24"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
@@ -2858,17 +2868,17 @@
     </row>
     <row r="32" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B32" s="8">
         <v>2</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="24"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
@@ -2881,17 +2891,17 @@
     </row>
     <row r="33" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B33" s="8">
         <v>3</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
-      <c r="F33" s="24"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -2904,17 +2914,17 @@
     </row>
     <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B34" s="8">
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
-      <c r="F34" s="24"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
@@ -2927,17 +2937,17 @@
     </row>
     <row r="35" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B35" s="8">
         <v>5</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="24"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
@@ -2950,17 +2960,17 @@
     </row>
     <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B36" s="8">
         <v>6</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="24"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
       <c r="I36" s="15"/>
@@ -2973,17 +2983,17 @@
     </row>
     <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B37" s="8">
         <v>7</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="24"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="15"/>
       <c r="H37" s="15"/>
       <c r="I37" s="15"/>
@@ -2996,14 +3006,14 @@
     </row>
     <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="24"/>
+      <c r="F38" s="23"/>
       <c r="G38" s="15"/>
       <c r="H38" s="15"/>
       <c r="I38" s="15"/>

</xml_diff>

<commit_message>
updated to dos and task parameters
</commit_message>
<xml_diff>
--- a/measures/word stimuli and task parameters.xlsx
+++ b/measures/word stimuli and task parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/irap-reliability-meta-analysis/measures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE34D32D-4FF0-EF48-8D4D-51BA320C1C76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B319E81D-6964-E542-B6D1-AAAC3366B2DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="460" windowWidth="23520" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="229">
   <si>
     <t>Religion</t>
   </si>
@@ -391,18 +391,6 @@
     <t>On the next block please respond AS IF DISGUSTING things are PLEASANT</t>
   </si>
   <si>
-    <t>Rubbish.jpg, Hand.jpg, Rat1.jpg, Mouth.jpg, Toilet1.jpg, Vomit.jpg</t>
-  </si>
-  <si>
-    <t>Bunny2.jpg, Kittens.jpg, Nature1.jpg, Puppy.jpg, Seal.jpg, Nature4.jpg</t>
-  </si>
-  <si>
-    <t>ik vind het vreselijk, ik vind dat het walgelijk is, het ziet er vies uit, ik voel me gedegouteerd, dat maakt me misselijk, ik ben geschokt</t>
-  </si>
-  <si>
-    <t>ik vind het plezierig, ik vind het fijn, het is goed, het maakt me gelukkig, het ziet er goed uit, het geeft me een zalig gevoel</t>
-  </si>
-  <si>
     <t>Friend-enemy</t>
   </si>
   <si>
@@ -410,12 +398,6 @@
   </si>
   <si>
     <t>During the next phase respond as if MEN are GENTLE and as if WOMEN are FORCEFUL. Please try to avoid the red X.</t>
-  </si>
-  <si>
-    <t>Hunger</t>
-  </si>
-  <si>
-    <t>Note that participants were assessed before lunchtime and had been instructed prior to participation to not eat breakfast, so that they had not eaten for 12+ hours.</t>
   </si>
   <si>
     <t>Personality</t>
@@ -672,6 +654,68 @@
   </si>
   <si>
     <t>females, women</t>
+  </si>
+  <si>
+    <t>Images taken from the International Affective Picture System (IAPS: Lang, Bradley, &amp; Cuthbert, 1997), which is proprietary and thereore cannot be distriuted here. Male picture numbers: 4460, 4500, 4534, 4550, 4561; female picture numbers: 4141, 4142, 4210, 4240, 4235.</t>
+  </si>
+  <si>
+    <t>happy, friendship, joy, peace, love, pleasure</t>
+  </si>
+  <si>
+    <t>Hitler, pedophile, cancer, incest, murder, suicide</t>
+  </si>
+  <si>
+    <t>good, pleasant, fun, positive, fantastic, excellent</t>
+  </si>
+  <si>
+    <t>bad, unpleasant, nasty, negative, horrible, terrible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same </t>
+  </si>
+  <si>
+    <t>Opposite</t>
+  </si>
+  <si>
+    <t>I find it horrible, I think it is disgusting, It looks nasty, I feel revolted, It makes me sick, I am repulsed</t>
+  </si>
+  <si>
+    <t>I think it’s pleasant, I find it nice, It’s good, It makes me feel happy, It looks nice, It makes me feel great</t>
+  </si>
+  <si>
+    <t>[pleasant images: baby, puppies, nature scenes, kittens, bunnies]</t>
+  </si>
+  <si>
+    <t>[disgusting images: rotten meat, a large maggot, bloody hand, diseased mouth cavity, toilet with feces, burned face]</t>
+  </si>
+  <si>
+    <t>Images taken from the International Affective Picture System and found online, see Hughes, Hussey, Corrigan, Jolie, Murphy &amp; Barnes-Holmes (2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During the next part of the experiment PLEASE RESPOND AS IF GOOD WORDS ARE GOOD AND BAD WORDS ARE BAD. </t>
+  </si>
+  <si>
+    <t>During the next part of the experiment PLEASE RESPOND AS IF GOOD WORDS ARE BAD AND BAD WORDS ARE GOOD.</t>
+  </si>
+  <si>
+    <t>Sexuality (1)</t>
+  </si>
+  <si>
+    <t>Sexuality (2)</t>
+  </si>
+  <si>
+    <t>Images taken from the International Affective Picture System (IAPS: Lang, Bradley, &amp; Cuthbert, 1997), which is proprietary and thereore cannot be distriuted here. Male picture numbers: 4460, 4500, 4534, 4550, 4561; female picture numbers: 4141, 4142, 4210, 4240, 4235.
+NB contains test-retest data</t>
+  </si>
+  <si>
+    <t>Disgust (2)</t>
+  </si>
+  <si>
+    <t>Disgust (1)</t>
+  </si>
+  <si>
+    <t>Images taken from the International Affective Picture System and found online, see Hughes, Hussey, Corrigan, Jolie, Murphy &amp; Barnes-Holmes (2016)
+NB contains test-retest data</t>
   </si>
 </sst>
 </file>
@@ -887,7 +931,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -956,6 +1000,16 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1427,10 +1481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1450,13 +1504,13 @@
   <sheetData>
     <row r="1" spans="1:16" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>18</v>
@@ -1465,7 +1519,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>54</v>
@@ -1595,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>99</v>
@@ -1642,7 +1696,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>106</v>
@@ -1689,7 +1743,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>89</v>
@@ -1736,7 +1790,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>96</v>
@@ -1783,7 +1837,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1830,7 +1884,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -1877,7 +1931,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -1916,13 +1970,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>110</v>
+        <v>227</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>119</v>
@@ -1943,16 +1999,16 @@
         <v>91</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>123</v>
+        <v>216</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>124</v>
+        <v>217</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>121</v>
+        <v>219</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>122</v>
+        <v>218</v>
       </c>
       <c r="N11" s="19" t="b">
         <v>1</v>
@@ -1961,46 +2017,48 @@
         <v>0</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>8</v>
+        <v>226</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>120</v>
       </c>
       <c r="F12" s="10">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G12" s="2">
         <v>2000</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>217</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>45</v>
+        <v>219</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>46</v>
+        <v>218</v>
       </c>
       <c r="N12" s="19" t="b">
         <v>1</v>
@@ -2008,124 +2066,148 @@
       <c r="O12" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="P12" s="19" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="F13" s="12">
-        <v>80</v>
-      </c>
-      <c r="G13" s="6">
+        <v>198</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="10">
+        <v>78</v>
+      </c>
+      <c r="G13" s="2">
         <v>2000</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="M13" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="N13" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="O13" s="20" t="b">
+      <c r="J13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N13" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O13" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="P13" s="21"/>
     </row>
     <row r="14" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="12">
+        <v>80</v>
+      </c>
+      <c r="G14" s="6">
+        <v>2000</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="M14" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="N14" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" s="21"/>
+    </row>
+    <row r="15" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="3">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="C15" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E15" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F15" s="10">
         <v>78</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G15" s="2">
         <v>2000</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N14" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="O14" s="19" t="b">
+      <c r="N15" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="19" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
@@ -2175,19 +2257,19 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F17" s="10">
         <v>78</v>
@@ -2202,13 +2284,13 @@
         <v>15</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M17" s="19" t="s">
         <v>60</v>
@@ -2220,24 +2302,24 @@
         <v>0</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F18" s="10">
         <v>78</v>
@@ -2252,16 +2334,16 @@
         <v>15</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="N18" s="19" t="b">
         <v>1</v>
@@ -2270,24 +2352,24 @@
         <v>0</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F19" s="10">
         <v>78</v>
@@ -2302,16 +2384,16 @@
         <v>15</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M19" s="19" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="N19" s="19" t="b">
         <v>1</v>
@@ -2320,24 +2402,24 @@
         <v>0</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F20" s="11">
         <v>78</v>
@@ -2352,16 +2434,16 @@
         <v>15</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="N20" s="19" t="b">
         <v>1</v>
@@ -2373,19 +2455,19 @@
     </row>
     <row r="21" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F21" s="11">
         <v>78</v>
@@ -2400,16 +2482,16 @@
         <v>15</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="N21" s="19" t="b">
         <v>1</v>
@@ -2420,19 +2502,19 @@
     </row>
     <row r="22" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F22" s="11">
         <v>78</v>
@@ -2447,16 +2529,16 @@
         <v>15</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="N22" s="19" t="b">
         <v>1</v>
@@ -2467,19 +2549,19 @@
     </row>
     <row r="23" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F23" s="11">
         <v>78</v>
@@ -2494,16 +2576,16 @@
         <v>15</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="N23" s="19" t="b">
         <v>1</v>
@@ -2514,19 +2596,19 @@
     </row>
     <row r="24" spans="1:16" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F24" s="11">
         <v>78</v>
@@ -2541,16 +2623,16 @@
         <v>15</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="N24" s="19" t="b">
         <v>1</v>
@@ -2567,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>3</v>
@@ -2614,7 +2696,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>13</v>
@@ -2664,7 +2746,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>13</v>
@@ -2703,7 +2785,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="68" customHeight="1" x14ac:dyDescent="0.2">
@@ -2795,13 +2877,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
       <c r="C30" s="3" t="s">
-        <v>111</v>
+        <v>223</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>112</v>
@@ -2818,7 +2902,7 @@
       <c r="H30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="J30" s="2" t="s">
@@ -2839,42 +2923,69 @@
       <c r="O30" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="P30" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B31" s="8">
-        <v>1</v>
+      <c r="P30" s="19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="3">
+        <v>2</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
+        <v>224</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="10">
+        <v>80</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2000</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="N31" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O31" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P31" s="19" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="32" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B32" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
@@ -2891,13 +3002,13 @@
     </row>
     <row r="33" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B33" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
@@ -2914,13 +3025,13 @@
     </row>
     <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B34" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
@@ -2937,13 +3048,13 @@
     </row>
     <row r="35" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B35" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
@@ -2960,13 +3071,13 @@
     </row>
     <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B36" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
@@ -2983,13 +3094,13 @@
     </row>
     <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B37" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
@@ -3006,10 +3117,13 @@
     </row>
     <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>177</v>
+        <v>170</v>
+      </c>
+      <c r="B38" s="8">
+        <v>7</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
@@ -3024,6 +3138,60 @@
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
     </row>
+    <row r="39" spans="1:15" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="24"/>
+      <c r="C39" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="F39" s="27">
+        <v>80</v>
+      </c>
+      <c r="G39" s="26">
+        <v>2000</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="K39" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="L39" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="M39" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="N39" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="O39" s="22" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D43"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Update word stimuli and task parameters.xlsx
</commit_message>
<xml_diff>
--- a/measures/word stimuli and task parameters.xlsx
+++ b/measures/word stimuli and task parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/irap-reliability-meta-analysis/measures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D41587-1A17-5449-B2F3-9DF6EE477438}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7266CF31-7578-AB48-8A61-A333033D12DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="460" windowWidth="23520" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="251">
   <si>
     <t>Religion</t>
   </si>
@@ -586,9 +586,6 @@
   </si>
   <si>
     <t>Shapes &amp; colors (1)</t>
-  </si>
-  <si>
-    <t>Shapes &amp; colors (2)</t>
   </si>
   <si>
     <t>Shapes &amp; colors (3)</t>
@@ -691,19 +688,12 @@
     <t>Disgust (1)</t>
   </si>
   <si>
-    <t>Images taken from the International Affective Picture System and found online, see Hughes, Hussey, Corrigan, Jolie, Murphy &amp; Barnes-Holmes (2016)
-NB contains test-retest data</t>
-  </si>
-  <si>
     <t>Trials per block</t>
   </si>
   <si>
     <t>Number of pairs of test blocks</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>corruption in Nigeria, exploitation in Bangladesh, discrimination in Pakistan, violence in Haiti, hunger in Zimbabwe, poverty in Uganda</t>
   </si>
   <si>
@@ -711,9 +701,6 @@
   </si>
   <si>
     <t>Basic education in Belgium, Extreme poverty in New Zealand, Safe drinking water in Sweden, Basic sanitation in Denmark, Vaccinations in Norway, Starving people in Canada</t>
-  </si>
-  <si>
-    <t>[whatever IRAP Emma used that predicted the BATs, as I have bat data!]</t>
   </si>
   <si>
     <t>True</t>
@@ -727,6 +714,73 @@
   </si>
   <si>
     <t>aggressive, dangerous, painful, rule, aggressive, dangerous, painful, rule</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>Green, Red, Blue, Green, Red, Blue</t>
+  </si>
+  <si>
+    <t>Triangle, Circle, Square, Triangle, Circle, Square</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Colours are colours and shapes are shapes</t>
+  </si>
+  <si>
+    <t>Colours are shapes and shapes are colours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respond correctly to the stimuli </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respond incorrectly to the stimuli </t>
+  </si>
+  <si>
+    <t>Respond as if colours are colours and shapes are shapes</t>
+  </si>
+  <si>
+    <t>Respond as if shapes are colours and colours are shapes</t>
+  </si>
+  <si>
+    <t>Please answer AS IF the word true is consistent and the word false is inconsistent</t>
+  </si>
+  <si>
+    <t>Please answer AS IF the word true is inconsistent and the word false is consistent</t>
+  </si>
+  <si>
+    <t>Stimuli identical to those used in Nicholson (REF)'s Disgust Sensitivity IRAP and were taken from the Images taken from the International Affective Picture System: "The picture numbers from the IAPs were as follows: 1111, 1205, 1280, 3250, 9300, 9373, 9405, 1440, 1463, 1710, 1750, 5201, 5250, 5731, 5760. The 16th pictorial stimulus was a photograph of Hitler which aimed to evoke socio-moral disgust."
+NB contains test-retest data</t>
+  </si>
+  <si>
+    <t>I Need to Look Away, I Need to Escape, I Worry I'll Get Sick, I Cannot Cope, I Worry I Might Faint, I Fear Contamination, I Fear Losing Control, I Cannot Tolerate It</t>
+  </si>
+  <si>
+    <t>I Can Look, I Can Stay, I Know I'll be Fine, I Can Tolerate It, I'm Sure I'll be OK, I Have No Fear, I Feel In Control, I Can Cope With This</t>
+  </si>
+  <si>
+    <t>On the next block please answer AS IF Disgusting things are Disgusting</t>
+  </si>
+  <si>
+    <t>On the next block please answer AS IF Disgusting things are Pleasant</t>
+  </si>
+  <si>
+    <t>Spiders2.jpg, Snakes.jpg, Rat1.jpg, Hand.jpg, Mouth.jpg, Toilet1.jpg, Vomit.jpg, adolf-hitler.jpg</t>
+  </si>
+  <si>
+    <t>Bunny2.jpg, Kittens.jpg, Nature1.jpg, Puppy.jpg, Seal.jpg, Nature2.jpg, Nature3.jpg, Nature4.jpg</t>
+  </si>
+  <si>
+    <t>Shapes &amp; colors (2)</t>
   </si>
 </sst>
 </file>
@@ -786,24 +840,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -948,7 +990,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -957,9 +999,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -986,9 +1025,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1010,21 +1046,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1032,7 +1064,28 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1504,82 +1557,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R42"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="18.83203125" style="7" customWidth="1"/>
-    <col min="4" max="5" width="32.5" style="8" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="33.1640625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="23" style="8" customWidth="1"/>
-    <col min="12" max="13" width="25" style="1" customWidth="1"/>
-    <col min="14" max="15" width="29" style="1" customWidth="1"/>
-    <col min="16" max="17" width="23.83203125" style="20" customWidth="1"/>
-    <col min="18" max="18" width="69.1640625" style="8" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="3" width="18.83203125" style="29" customWidth="1"/>
+    <col min="4" max="5" width="32.5" style="26" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" style="30" customWidth="1"/>
+    <col min="9" max="9" width="33.1640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="23" style="26" customWidth="1"/>
+    <col min="12" max="13" width="25" style="28" customWidth="1"/>
+    <col min="14" max="15" width="29" style="28" customWidth="1"/>
+    <col min="16" max="17" width="23.83203125" style="25" customWidth="1"/>
+    <col min="18" max="18" width="69.1640625" style="26" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:18" s="27" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="F1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="P1" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1597,13 +1650,13 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="15">
         <v>24</v>
       </c>
-      <c r="G2" s="17">
-        <v>3</v>
-      </c>
-      <c r="H2" s="9">
+      <c r="G2" s="15">
+        <v>3</v>
+      </c>
+      <c r="H2" s="8">
         <v>80</v>
       </c>
       <c r="I2" s="2">
@@ -1627,33 +1680,35 @@
       <c r="O2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q2" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P2" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R2" s="7"/>
     </row>
     <row r="3" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="15">
         <v>24</v>
       </c>
-      <c r="G3" s="20">
-        <v>3</v>
-      </c>
-      <c r="H3" s="9">
+      <c r="G3" s="18">
+        <v>3</v>
+      </c>
+      <c r="H3" s="8">
         <v>78</v>
       </c>
       <c r="I3" s="2">
@@ -1671,51 +1726,52 @@
       <c r="M3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="15" t="s">
         <v>69</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P3" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q3" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P3" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R3" s="7"/>
     </row>
     <row r="4" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="15">
         <v>24</v>
       </c>
-      <c r="G4" s="20">
-        <v>3</v>
-      </c>
-      <c r="H4" s="10">
+      <c r="G4" s="18">
+        <v>3</v>
+      </c>
+      <c r="H4" s="9">
         <v>80</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>2000</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -1730,45 +1786,46 @@
       <c r="O4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="P4" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q4" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P4" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R4" s="7"/>
     </row>
     <row r="5" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="15">
         <v>24</v>
       </c>
-      <c r="G5" s="20">
-        <v>3</v>
-      </c>
-      <c r="H5" s="10">
+      <c r="G5" s="18">
+        <v>3</v>
+      </c>
+      <c r="H5" s="9">
         <v>80</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>2000</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -1778,50 +1835,51 @@
         <v>99</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="P5" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q5" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P5" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="15">
         <v>24</v>
       </c>
-      <c r="G6" s="20">
-        <v>3</v>
-      </c>
-      <c r="H6" s="10">
+      <c r="G6" s="18">
+        <v>3</v>
+      </c>
+      <c r="H6" s="9">
         <v>80</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>2000</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -1836,45 +1894,46 @@
       <c r="O6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P6" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q6" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P6" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R6" s="7"/>
     </row>
     <row r="7" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="15">
         <v>24</v>
       </c>
-      <c r="G7" s="20">
-        <v>3</v>
-      </c>
-      <c r="H7" s="10">
+      <c r="G7" s="18">
+        <v>3</v>
+      </c>
+      <c r="H7" s="9">
         <v>80</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>2000</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -1884,17 +1943,18 @@
         <v>91</v>
       </c>
       <c r="N7" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q7" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="P7" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q7" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="R7" s="7"/>
     </row>
     <row r="8" spans="1:18" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -1912,13 +1972,13 @@
       <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="15">
         <v>24</v>
       </c>
-      <c r="G8" s="17">
-        <v>3</v>
-      </c>
-      <c r="H8" s="9">
+      <c r="G8" s="15">
+        <v>3</v>
+      </c>
+      <c r="H8" s="8">
         <v>80</v>
       </c>
       <c r="I8" s="2">
@@ -1927,7 +1987,7 @@
       <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1942,12 +2002,13 @@
       <c r="O8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q8" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P8" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q8" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:18" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1965,13 +2026,13 @@
       <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="15">
         <v>24</v>
       </c>
-      <c r="G9" s="17">
-        <v>3</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="G9" s="15">
+        <v>3</v>
+      </c>
+      <c r="H9" s="8">
         <v>80</v>
       </c>
       <c r="I9" s="2">
@@ -1980,7 +2041,7 @@
       <c r="J9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L9" s="1" t="s">
@@ -1995,12 +2056,13 @@
       <c r="O9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P9" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q9" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P9" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q9" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="1:18" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -2018,13 +2080,13 @@
       <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="15">
         <v>24</v>
       </c>
-      <c r="G10" s="17">
-        <v>3</v>
-      </c>
-      <c r="H10" s="9">
+      <c r="G10" s="15">
+        <v>3</v>
+      </c>
+      <c r="H10" s="8">
         <v>80</v>
       </c>
       <c r="I10" s="2">
@@ -2033,7 +2095,7 @@
       <c r="J10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -2048,14 +2110,15 @@
       <c r="O10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="P10" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q10" s="28" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P10" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q10" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="1:18" ht="122" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>105</v>
       </c>
@@ -2063,21 +2126,21 @@
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F11" s="17">
+        <v>219</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="15">
         <v>32</v>
       </c>
-      <c r="G11" s="20">
-        <v>3</v>
-      </c>
-      <c r="H11" s="9">
+      <c r="G11" s="18">
+        <v>3</v>
+      </c>
+      <c r="H11" s="8">
         <v>80</v>
       </c>
       <c r="I11" s="2">
@@ -2086,23 +2149,29 @@
       <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q11" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>221</v>
+      <c r="L11" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="N11" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="O11" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="P11" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.2">
@@ -2113,21 +2182,21 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D12" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="15">
         <v>24</v>
       </c>
-      <c r="G12" s="20">
-        <v>3</v>
-      </c>
-      <c r="H12" s="9">
+      <c r="G12" s="18">
+        <v>3</v>
+      </c>
+      <c r="H12" s="8">
         <v>80</v>
       </c>
       <c r="I12" s="2">
@@ -2136,29 +2205,29 @@
       <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="L12" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="M12" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="N12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="P12" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q12" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R12" s="15" t="s">
         <v>212</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="P12" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q12" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R12" s="17" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -2167,7 +2236,7 @@
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>7</v>
@@ -2175,13 +2244,13 @@
       <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="15">
         <v>24</v>
       </c>
-      <c r="G13" s="17">
-        <v>3</v>
-      </c>
-      <c r="H13" s="9">
+      <c r="G13" s="15">
+        <v>3</v>
+      </c>
+      <c r="H13" s="8">
         <v>78</v>
       </c>
       <c r="I13" s="2">
@@ -2205,12 +2274,13 @@
       <c r="O13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q13" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P13" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q13" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R13" s="7"/>
     </row>
     <row r="14" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -2222,49 +2292,49 @@
       <c r="C14" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="15">
         <v>24</v>
       </c>
-      <c r="G14" s="20">
-        <v>3</v>
-      </c>
-      <c r="H14" s="11">
+      <c r="G14" s="18">
+        <v>3</v>
+      </c>
+      <c r="H14" s="10">
         <v>80</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>2000</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="M14" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="M14" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="N14" s="18" t="s">
+      <c r="N14" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="O14" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="O14" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="P14" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q14" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R14" s="19"/>
+      <c r="P14" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q14" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R14" s="17"/>
     </row>
     <row r="15" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -2276,19 +2346,19 @@
       <c r="C15" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="15">
         <v>24</v>
       </c>
-      <c r="G15" s="20">
-        <v>3</v>
-      </c>
-      <c r="H15" s="9">
+      <c r="G15" s="18">
+        <v>3</v>
+      </c>
+      <c r="H15" s="8">
         <v>78</v>
       </c>
       <c r="I15" s="2">
@@ -2312,12 +2382,13 @@
       <c r="O15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P15" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q15" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P15" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q15" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" spans="1:18" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -2333,13 +2404,13 @@
       <c r="E16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="15">
         <v>24</v>
       </c>
-      <c r="G16" s="17">
-        <v>3</v>
-      </c>
-      <c r="H16" s="9">
+      <c r="G16" s="15">
+        <v>3</v>
+      </c>
+      <c r="H16" s="8">
         <v>78</v>
       </c>
       <c r="I16" s="1">
@@ -2363,14 +2434,15 @@
       <c r="O16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P16" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q16" s="28" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="P16" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q16" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R16" s="7"/>
+    </row>
+    <row r="17" spans="1:18" s="28" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>127</v>
       </c>
@@ -2378,7 +2450,7 @@
         <v>57</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>128</v>
@@ -2386,19 +2458,19 @@
       <c r="E17" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="15">
         <v>32</v>
       </c>
-      <c r="G17" s="17">
-        <v>3</v>
-      </c>
-      <c r="H17" s="9">
+      <c r="G17" s="15">
+        <v>3</v>
+      </c>
+      <c r="H17" s="8">
         <v>78</v>
       </c>
       <c r="I17" s="1">
         <v>2000</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="15" t="s">
         <v>17</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -2410,31 +2482,31 @@
       <c r="M17" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N17" s="17" t="s">
+      <c r="N17" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="O17" s="17" t="s">
+      <c r="O17" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="P17" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q17" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R17" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="P17" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q17" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="28" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>125</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>128</v>
@@ -2442,19 +2514,19 @@
       <c r="E18" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="15">
         <v>32</v>
       </c>
-      <c r="G18" s="17">
-        <v>3</v>
-      </c>
-      <c r="H18" s="9">
+      <c r="G18" s="15">
+        <v>3</v>
+      </c>
+      <c r="H18" s="8">
         <v>78</v>
       </c>
       <c r="I18" s="1">
         <v>2000</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="15" t="s">
         <v>17</v>
       </c>
       <c r="K18" s="1" t="s">
@@ -2466,31 +2538,31 @@
       <c r="M18" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N18" s="17" t="s">
+      <c r="N18" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="O18" s="17" t="s">
+      <c r="O18" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="P18" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q18" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R18" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="P18" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q18" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R18" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="28" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>126</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>128</v>
@@ -2498,19 +2570,19 @@
       <c r="E19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="15">
         <v>32</v>
       </c>
-      <c r="G19" s="17">
-        <v>3</v>
-      </c>
-      <c r="H19" s="9">
+      <c r="G19" s="15">
+        <v>3</v>
+      </c>
+      <c r="H19" s="8">
         <v>78</v>
       </c>
       <c r="I19" s="1">
         <v>2000</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="15" t="s">
         <v>17</v>
       </c>
       <c r="K19" s="1" t="s">
@@ -2522,20 +2594,20 @@
       <c r="M19" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N19" s="17" t="s">
+      <c r="N19" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="O19" s="17" t="s">
+      <c r="O19" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="P19" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q19" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R19" s="17" t="s">
-        <v>197</v>
+      <c r="P19" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q19" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R19" s="15" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="55" customHeight="1" x14ac:dyDescent="0.2">
@@ -2548,25 +2620,25 @@
       <c r="C20" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="15">
         <v>24</v>
       </c>
-      <c r="G20" s="20">
-        <v>3</v>
-      </c>
-      <c r="H20" s="10">
+      <c r="G20" s="18">
+        <v>3</v>
+      </c>
+      <c r="H20" s="9">
         <v>78</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="7">
         <v>2500</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -2584,13 +2656,13 @@
       <c r="O20" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="P20" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q20" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R20" s="20"/>
+      <c r="P20" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q20" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="1:18" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
@@ -2602,25 +2674,25 @@
       <c r="C21" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="15">
         <v>24</v>
       </c>
-      <c r="G21" s="20">
-        <v>3</v>
-      </c>
-      <c r="H21" s="10">
+      <c r="G21" s="18">
+        <v>3</v>
+      </c>
+      <c r="H21" s="9">
         <v>78</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="7">
         <v>2500</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K21" s="1" t="s">
@@ -2638,12 +2710,13 @@
       <c r="O21" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="P21" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q21" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P21" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q21" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R21" s="7"/>
     </row>
     <row r="22" spans="1:18" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -2655,25 +2728,25 @@
       <c r="C22" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="15">
         <v>24</v>
       </c>
-      <c r="G22" s="20">
-        <v>3</v>
-      </c>
-      <c r="H22" s="10">
+      <c r="G22" s="18">
+        <v>3</v>
+      </c>
+      <c r="H22" s="9">
         <v>78</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="7">
         <v>2500</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -2691,12 +2764,13 @@
       <c r="O22" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="P22" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q22" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P22" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q22" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R22" s="7"/>
     </row>
     <row r="23" spans="1:18" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -2708,25 +2782,25 @@
       <c r="C23" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="15">
         <v>24</v>
       </c>
-      <c r="G23" s="20">
-        <v>3</v>
-      </c>
-      <c r="H23" s="10">
+      <c r="G23" s="18">
+        <v>3</v>
+      </c>
+      <c r="H23" s="9">
         <v>78</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="7">
         <v>2500</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K23" s="1" t="s">
@@ -2744,12 +2818,13 @@
       <c r="O23" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="P23" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q23" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P23" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q23" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R23" s="7"/>
     </row>
     <row r="24" spans="1:18" ht="55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -2761,25 +2836,25 @@
       <c r="C24" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="15">
         <v>24</v>
       </c>
-      <c r="G24" s="20">
-        <v>3</v>
-      </c>
-      <c r="H24" s="10">
+      <c r="G24" s="18">
+        <v>3</v>
+      </c>
+      <c r="H24" s="9">
         <v>78</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="7">
         <v>2500</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K24" s="1" t="s">
@@ -2797,12 +2872,13 @@
       <c r="O24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P24" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q24" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P24" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q24" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R24" s="7"/>
     </row>
     <row r="25" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -2820,13 +2896,13 @@
       <c r="E25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="15">
         <v>24</v>
       </c>
-      <c r="G25" s="17">
-        <v>3</v>
-      </c>
-      <c r="H25" s="9">
+      <c r="G25" s="15">
+        <v>3</v>
+      </c>
+      <c r="H25" s="8">
         <v>80</v>
       </c>
       <c r="I25" s="1">
@@ -2850,12 +2926,13 @@
       <c r="O25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P25" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q25" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P25" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q25" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R25" s="7"/>
     </row>
     <row r="26" spans="1:18" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
@@ -2867,19 +2944,19 @@
       <c r="C26" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="15">
         <v>32</v>
       </c>
-      <c r="G26" s="17">
-        <v>3</v>
-      </c>
-      <c r="H26" s="9">
+      <c r="G26" s="15">
+        <v>3</v>
+      </c>
+      <c r="H26" s="8">
         <v>80</v>
       </c>
       <c r="I26" s="2">
@@ -2888,7 +2965,7 @@
       <c r="J26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K26" s="8" t="s">
+      <c r="K26" s="7" t="s">
         <v>89</v>
       </c>
       <c r="L26" s="1" t="s">
@@ -2898,18 +2975,18 @@
         <v>54</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="P26" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q26" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R26" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q26" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R26" s="15" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2927,13 +3004,13 @@
       <c r="E27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="15">
         <v>24</v>
       </c>
-      <c r="G27" s="17">
-        <v>3</v>
-      </c>
-      <c r="H27" s="9">
+      <c r="G27" s="15">
+        <v>3</v>
+      </c>
+      <c r="H27" s="8">
         <v>80</v>
       </c>
       <c r="I27" s="1">
@@ -2957,33 +3034,35 @@
       <c r="O27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P27" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q27" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P27" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q27" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R27" s="7"/>
     </row>
     <row r="28" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="B28" s="6"/>
       <c r="C28" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="15">
         <v>24</v>
       </c>
-      <c r="G28" s="20">
-        <v>3</v>
-      </c>
-      <c r="H28" s="9">
+      <c r="G28" s="18">
+        <v>3</v>
+      </c>
+      <c r="H28" s="8">
         <v>78</v>
       </c>
       <c r="I28" s="2">
@@ -3007,12 +3086,13 @@
       <c r="O28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P28" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q28" s="28" t="s">
-        <v>230</v>
-      </c>
+      <c r="P28" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q28" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R28" s="7"/>
     </row>
     <row r="29" spans="1:18" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
@@ -3022,21 +3102,21 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D29" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F29" s="15">
         <v>40</v>
       </c>
-      <c r="G29" s="20">
-        <v>3</v>
-      </c>
-      <c r="H29" s="9">
+      <c r="G29" s="18">
+        <v>3</v>
+      </c>
+      <c r="H29" s="8">
         <v>80</v>
       </c>
       <c r="I29" s="2">
@@ -3045,7 +3125,7 @@
       <c r="J29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K29" s="17" t="s">
+      <c r="K29" s="15" t="s">
         <v>15</v>
       </c>
       <c r="L29" s="2" t="s">
@@ -3060,14 +3140,14 @@
       <c r="O29" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P29" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q29" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R29" s="17" t="s">
-        <v>218</v>
+      <c r="P29" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q29" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R29" s="15" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="67" customHeight="1" x14ac:dyDescent="0.2">
@@ -3078,21 +3158,21 @@
         <v>2</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D30" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="15">
         <v>40</v>
       </c>
-      <c r="G30" s="20">
-        <v>3</v>
-      </c>
-      <c r="H30" s="9">
+      <c r="G30" s="18">
+        <v>3</v>
+      </c>
+      <c r="H30" s="8">
         <v>80</v>
       </c>
       <c r="I30" s="2">
@@ -3101,7 +3181,7 @@
       <c r="J30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="17" t="s">
+      <c r="K30" s="15" t="s">
         <v>15</v>
       </c>
       <c r="L30" s="2" t="s">
@@ -3116,278 +3196,445 @@
       <c r="O30" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P30" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="Q30" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="R30" s="17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="P30" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q30" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R30" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="6">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="G31" s="13">
-        <v>3</v>
-      </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="29"/>
-      <c r="Q31" s="29"/>
-    </row>
-    <row r="32" spans="1:18" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="D31" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="F31" s="15">
+        <v>24</v>
+      </c>
+      <c r="G31" s="18">
+        <v>3</v>
+      </c>
+      <c r="H31" s="8">
+        <v>80</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="N31" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="O31" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="P31" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q31" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="R31" s="7"/>
+    </row>
+    <row r="32" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="7">
-        <v>2</v>
+      <c r="B32" s="6">
+        <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="F32" s="15">
+        <v>24</v>
+      </c>
+      <c r="G32" s="18">
+        <v>3</v>
+      </c>
+      <c r="H32" s="8">
+        <v>80</v>
+      </c>
+      <c r="I32" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L32" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="P32" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q32" s="31" t="s">
+        <v>234</v>
+      </c>
+      <c r="R32" s="7"/>
+    </row>
+    <row r="33" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B33" s="6">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="G32" s="13">
-        <v>3</v>
-      </c>
-      <c r="H32" s="21"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
-    </row>
-    <row r="33" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="D33" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="F33" s="15">
+        <v>24</v>
+      </c>
+      <c r="G33" s="18">
+        <v>3</v>
+      </c>
+      <c r="H33" s="8">
+        <v>80</v>
+      </c>
+      <c r="I33" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="M33" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="P33" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q33" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R33" s="7"/>
+    </row>
+    <row r="34" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="7">
-        <v>3</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B34" s="6">
+        <v>4</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="G33" s="13">
-        <v>3</v>
-      </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="29"/>
-      <c r="Q33" s="29"/>
-    </row>
-    <row r="34" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="D34" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="F34" s="15">
+        <v>24</v>
+      </c>
+      <c r="G34" s="18">
+        <v>3</v>
+      </c>
+      <c r="H34" s="8">
+        <v>80</v>
+      </c>
+      <c r="I34" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="M34" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="N34" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="O34" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="P34" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q34" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="7">
-        <v>4</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B35" s="6">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="G34" s="13">
-        <v>3</v>
-      </c>
-      <c r="H34" s="21"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="29"/>
-      <c r="Q34" s="29"/>
-    </row>
-    <row r="35" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="D35" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="F35" s="15">
+        <v>24</v>
+      </c>
+      <c r="G35" s="18">
+        <v>3</v>
+      </c>
+      <c r="H35" s="8">
+        <v>80</v>
+      </c>
+      <c r="I35" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="N35" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="P35" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q35" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R35" s="7"/>
+    </row>
+    <row r="36" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="7">
-        <v>5</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B36" s="6">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="G35" s="13">
-        <v>3</v>
-      </c>
-      <c r="H35" s="21"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-    </row>
-    <row r="36" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="D36" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="F36" s="15">
+        <v>24</v>
+      </c>
+      <c r="G36" s="18">
+        <v>3</v>
+      </c>
+      <c r="H36" s="8">
+        <v>80</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="M36" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="N36" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="O36" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="P36" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q36" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R36" s="7"/>
+    </row>
+    <row r="37" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B36" s="7">
-        <v>6</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B37" s="6">
+        <v>7</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="G36" s="13">
-        <v>3</v>
-      </c>
-      <c r="H36" s="21"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="29"/>
-    </row>
-    <row r="37" spans="1:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B37" s="7">
-        <v>7</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="G37" s="13">
-        <v>3</v>
-      </c>
-      <c r="H37" s="21"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="29"/>
-      <c r="Q37" s="29"/>
-    </row>
-    <row r="38" spans="1:17" s="20" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
+      <c r="D37" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F37" s="15">
+        <v>24</v>
+      </c>
+      <c r="G37" s="18">
+        <v>3</v>
+      </c>
+      <c r="H37" s="8">
+        <v>80</v>
+      </c>
+      <c r="I37" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="N37" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="O37" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="P37" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q37" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="R37" s="7"/>
+    </row>
+    <row r="38" spans="1:18" s="25" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="23" t="s">
+      <c r="B38" s="19"/>
+      <c r="C38" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="D38" s="24" t="s">
+      <c r="D38" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="E38" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="E38" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="F38" s="17">
+      <c r="F38" s="15">
         <v>24</v>
       </c>
-      <c r="G38" s="20">
-        <v>3</v>
-      </c>
-      <c r="H38" s="25">
+      <c r="G38" s="18">
+        <v>3</v>
+      </c>
+      <c r="H38" s="21">
         <v>80</v>
       </c>
-      <c r="I38" s="24">
+      <c r="I38" s="18">
         <v>2000</v>
       </c>
-      <c r="J38" s="20" t="s">
+      <c r="J38" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="K38" s="20" t="s">
+      <c r="K38" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="L38" s="17" t="s">
+      <c r="L38" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="M38" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="M38" s="17" t="s">
+      <c r="N38" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="N38" s="27" t="s">
+      <c r="O38" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="O38" s="17" t="s">
+      <c r="P38" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="P38" s="20" t="s">
+      <c r="Q38" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="Q38" s="20" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D40"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D42"/>
+      <c r="R38" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>